<commit_message>
Changes to feature slides
</commit_message>
<xml_diff>
--- a/Technical Report/Model Selection.xlsx
+++ b/Technical Report/Model Selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Documents\Capstone-Reviews-Ranker\Technical Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004CF2D9-F323-473C-AA8C-138E7E56662C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FB90D8-4D74-4BF2-A56A-801978385D74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acronyms" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Laptop" sheetId="3" r:id="rId3"/>
     <sheet name="Camera" sheetId="4" r:id="rId4"/>
     <sheet name="Model Select" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="7" state="hidden" r:id="rId6"/>
-    <sheet name="RF" sheetId="5" r:id="rId7"/>
+    <sheet name="RF" sheetId="7" r:id="rId6"/>
+    <sheet name="SVM" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="77">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -292,7 +292,8 @@
     <t>h</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Average Across
+Product Groups</t>
   </si>
 </sst>
 </file>
@@ -330,7 +331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,8 +350,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -373,11 +380,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -411,9 +427,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -422,8 +435,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893ACE32-00B3-467D-9D40-144FA6224D42}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -720,148 +760,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>75</v>
       </c>
     </row>
@@ -899,18 +939,18 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1528,18 +1568,18 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -2171,18 +2211,18 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -2790,10 +2830,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B49362D-4B66-4F22-8BDC-B2ED18289D06}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2953,495 +2996,590 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69C8DED-F07A-4836-BFB4-627A7E0EB61D}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="24" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="13">
         <v>14.02</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="13">
         <v>14.69</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="13">
         <v>12.43</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="20">
         <f>AVERAGE(C3:E3)</f>
         <v>13.713333333333333</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="13">
+        <f>MAX(C3:E3)-MIN(C3:E3)</f>
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="13">
         <v>14.43</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="13">
         <v>14.6</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="13">
         <v>12.68</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="20">
         <f t="shared" ref="F4:F22" si="0">AVERAGE(C4:E4)</f>
         <v>13.903333333333334</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="13">
+        <f t="shared" ref="G4:G22" si="1">MAX(C4:E4)-MIN(C4:E4)</f>
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="13">
         <v>15.09</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="13">
         <v>14.9</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="13">
         <v>12.6</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="20">
         <f t="shared" si="0"/>
         <v>14.196666666666667</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="13">
+        <f t="shared" si="1"/>
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="13">
         <v>14.08</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="13">
         <v>14.88</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="13">
         <v>12.51</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="20">
         <f t="shared" si="0"/>
         <v>13.823333333333332</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="13">
+        <f t="shared" si="1"/>
+        <v>2.370000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="13">
         <v>13.19</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="13">
         <v>15.04</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="21">
         <v>12.3</v>
       </c>
-      <c r="F7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="20">
+        <f t="shared" si="0"/>
+        <v>13.51</v>
+      </c>
+      <c r="G7" s="13">
+        <f t="shared" si="1"/>
+        <v>2.7399999999999984</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="13">
         <v>14.9</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="13">
         <v>15.8</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="13">
         <v>12.64</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="20">
         <f t="shared" si="0"/>
         <v>14.446666666666667</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="13">
+        <f t="shared" si="1"/>
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="13">
         <v>14.8</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="13">
         <v>15.66</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="13">
         <v>12.7</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="20">
         <f t="shared" si="0"/>
         <v>14.386666666666665</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="13">
+        <f t="shared" si="1"/>
+        <v>2.9600000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="13">
         <v>14.86</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="13">
         <v>15.6</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="13">
         <v>13.21</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="20">
         <f t="shared" si="0"/>
         <v>14.556666666666667</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="13">
+        <f t="shared" si="1"/>
+        <v>2.3899999999999988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="13">
         <v>15.4</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="13">
         <v>14.55</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="13">
         <v>12.5</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="20">
         <f t="shared" si="0"/>
         <v>14.15</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="13">
+        <f t="shared" si="1"/>
+        <v>2.9000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="13">
         <v>14.98</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="13">
         <v>14.92</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="13">
         <v>12.33</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="20">
         <f t="shared" si="0"/>
         <v>14.076666666666666</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="13">
+        <f t="shared" si="1"/>
+        <v>2.6500000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="13">
         <v>14.81</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="13">
         <v>14.64</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="13">
         <v>12.38</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="20">
         <f t="shared" si="0"/>
         <v>13.943333333333335</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="13">
+        <f t="shared" si="1"/>
+        <v>2.4299999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="13">
         <v>14.78</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="13">
         <v>14.79</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="13">
         <v>12.51</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="20">
         <f t="shared" si="0"/>
         <v>14.026666666666666</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="13">
+        <f t="shared" si="1"/>
+        <v>2.2799999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="13">
         <v>13.62</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="13">
         <v>14.72</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="13">
         <v>12.6</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="20">
         <f t="shared" si="0"/>
         <v>13.646666666666667</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="13">
+        <f t="shared" si="1"/>
+        <v>2.120000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="13">
         <v>13.37</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="13">
         <v>16.010000000000002</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="13">
         <v>12.64</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="20">
         <f t="shared" si="0"/>
         <v>14.006666666666668</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="13">
+        <f t="shared" si="1"/>
+        <v>3.370000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="13">
         <v>13.65</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="13">
         <v>14.81</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="13">
         <v>12.7</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="20">
         <f t="shared" si="0"/>
         <v>13.719999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="13">
+        <f t="shared" si="1"/>
+        <v>2.1100000000000012</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="13">
         <v>13.52</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="13">
         <v>15.78</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="13">
         <v>12.86</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="20">
         <f t="shared" si="0"/>
         <v>14.053333333333333</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="G18" s="13">
+        <f t="shared" si="1"/>
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
         <v>17</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="22">
         <v>13.27</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="22">
         <v>14.22</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="22">
         <v>13.05</v>
       </c>
-      <c r="F19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="23">
+        <f t="shared" si="0"/>
+        <v>13.513333333333335</v>
+      </c>
+      <c r="G19" s="22">
+        <f t="shared" si="1"/>
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="13">
         <v>12.95</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="13">
         <v>15.9</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="13">
         <v>12.94</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="20">
         <f t="shared" si="0"/>
         <v>13.93</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="13">
+        <f t="shared" si="1"/>
+        <v>2.9600000000000009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="13">
         <v>13.21</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="13">
         <v>15.48</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="13">
         <v>13.1</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="20">
         <f t="shared" si="0"/>
         <v>13.93</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="13">
+        <f t="shared" si="1"/>
+        <v>2.3800000000000008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="21">
         <v>12.85</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="14">
         <v>15.78</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="14">
         <v>12.88</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="20">
         <f t="shared" si="0"/>
         <v>13.836666666666666</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="13">
+        <f t="shared" si="1"/>
+        <v>2.9299999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C24">
-        <f t="shared" ref="C24:E24" si="1">MIN(C3:C22)</f>
+        <f t="shared" ref="C24:E24" si="2">MIN(C3:C22)</f>
         <v>12.85</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.22</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.3</v>
       </c>
       <c r="F24">
         <f>MIN(F3:F22)</f>
-        <v>13.646666666666667</v>
+        <v>13.51</v>
+      </c>
+      <c r="G24">
+        <f>MIN(G3:G22)</f>
+        <v>1.17</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB77A860-CAB5-4F23-8E3E-3552D28E08A7}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>